<commit_message>
Update to checklist regarding input_read_count field
</commit_message>
<xml_diff>
--- a/input/FAIRe_NOAA_checklist_v1.0.xlsx
+++ b/input/FAIRe_NOAA_checklist_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayden.willms\Documents\Code\FAIReSheets\FAIReSheets\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6AA19E-41F0-4834-8132-F57FDC0D7961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF30A36-85DD-4A43-B8A0-47BC61B311DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33105" yWindow="1155" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="2325" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4110" uniqueCount="1359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4109" uniqueCount="1358">
   <si>
     <t>Instructions for data submitters:</t>
   </si>
@@ -4077,9 +4077,6 @@
   </si>
   <si>
     <t>NOAAanalysisMetadata</t>
-  </si>
-  <si>
-    <t>Anything below this line is essentially a change to the original FAIRe Checklist</t>
   </si>
   <si>
     <t>deblur_min_size</t>
@@ -4104,7 +4101,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4133,14 +4130,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4207,12 +4198,6 @@
         <fgColor rgb="FFCCFF99"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4226,7 +4211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4242,8 +4227,6 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4708,10 +4691,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P409"/>
+  <dimension ref="A1:P408"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C363" sqref="C363"/>
+    <sheetView tabSelected="1" topLeftCell="A272" workbookViewId="0">
+      <selection activeCell="D311" sqref="D311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15132,19 +15115,24 @@
       </c>
     </row>
     <row r="302" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A302" s="15" t="s">
-        <v>1352</v>
-      </c>
-      <c r="B302" s="16"/>
-      <c r="C302" s="15"/>
-      <c r="D302" s="15"/>
-      <c r="E302" s="15"/>
-      <c r="F302" s="15"/>
-      <c r="G302" s="15"/>
-      <c r="H302" s="15"/>
-      <c r="I302" s="15"/>
-      <c r="J302" s="15"/>
-      <c r="K302" s="15"/>
+      <c r="A302" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B302" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>1282</v>
+      </c>
+      <c r="E302" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F302" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="N302" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="303" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
@@ -15154,7 +15142,7 @@
         <v>53</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="E303" s="12" t="s">
         <v>64</v>
@@ -15174,7 +15162,7 @@
         <v>53</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="E304" s="12" t="s">
         <v>64</v>
@@ -15194,7 +15182,7 @@
         <v>53</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="E305" s="12" t="s">
         <v>64</v>
@@ -15208,13 +15196,13 @@
     </row>
     <row r="306" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>1346</v>
-      </c>
-      <c r="B306" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C306" s="1" t="s">
-        <v>1285</v>
+        <v>1347</v>
+      </c>
+      <c r="B306" s="7" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C306" s="14" t="s">
+        <v>1286</v>
       </c>
       <c r="E306" s="12" t="s">
         <v>64</v>
@@ -15234,7 +15222,7 @@
         <v>1032</v>
       </c>
       <c r="C307" s="14" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="E307" s="12" t="s">
         <v>64</v>
@@ -15254,7 +15242,7 @@
         <v>1032</v>
       </c>
       <c r="C308" s="14" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="E308" s="12" t="s">
         <v>64</v>
@@ -15274,7 +15262,7 @@
         <v>1032</v>
       </c>
       <c r="C309" s="14" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="E309" s="12" t="s">
         <v>64</v>
@@ -15294,7 +15282,7 @@
         <v>1032</v>
       </c>
       <c r="C310" s="14" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="E310" s="12" t="s">
         <v>64</v>
@@ -15314,7 +15302,7 @@
         <v>1032</v>
       </c>
       <c r="C311" s="14" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="E311" s="12" t="s">
         <v>64</v>
@@ -15334,7 +15322,7 @@
         <v>1032</v>
       </c>
       <c r="C312" s="14" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="E312" s="12" t="s">
         <v>64</v>
@@ -15354,7 +15342,7 @@
         <v>1032</v>
       </c>
       <c r="C313" s="14" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="E313" s="12" t="s">
         <v>64</v>
@@ -15370,11 +15358,8 @@
       <c r="A314" t="s">
         <v>1347</v>
       </c>
-      <c r="B314" s="7" t="s">
-        <v>1032</v>
-      </c>
       <c r="C314" s="14" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="E314" s="12" t="s">
         <v>64</v>
@@ -15390,8 +15375,11 @@
       <c r="A315" t="s">
         <v>1347</v>
       </c>
+      <c r="B315" s="7" t="s">
+        <v>1032</v>
+      </c>
       <c r="C315" s="14" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="E315" s="12" t="s">
         <v>64</v>
@@ -15411,7 +15399,7 @@
         <v>1032</v>
       </c>
       <c r="C316" s="14" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="E316" s="12" t="s">
         <v>64</v>
@@ -15431,7 +15419,7 @@
         <v>1032</v>
       </c>
       <c r="C317" s="14" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="E317" s="12" t="s">
         <v>64</v>
@@ -15451,7 +15439,7 @@
         <v>1032</v>
       </c>
       <c r="C318" s="14" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="E318" s="12" t="s">
         <v>64</v>
@@ -15471,7 +15459,7 @@
         <v>1032</v>
       </c>
       <c r="C319" s="14" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="E319" s="12" t="s">
         <v>64</v>
@@ -15491,7 +15479,7 @@
         <v>1032</v>
       </c>
       <c r="C320" s="14" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="E320" s="12" t="s">
         <v>64</v>
@@ -15511,7 +15499,7 @@
         <v>1032</v>
       </c>
       <c r="C321" s="14" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="E321" s="12" t="s">
         <v>64</v>
@@ -15531,7 +15519,7 @@
         <v>1032</v>
       </c>
       <c r="C322" s="14" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="E322" s="12" t="s">
         <v>64</v>
@@ -15551,7 +15539,7 @@
         <v>1032</v>
       </c>
       <c r="C323" s="14" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="E323" s="12" t="s">
         <v>64</v>
@@ -15571,7 +15559,7 @@
         <v>1032</v>
       </c>
       <c r="C324" s="14" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="E324" s="12" t="s">
         <v>64</v>
@@ -15591,7 +15579,7 @@
         <v>1032</v>
       </c>
       <c r="C325" s="14" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="E325" s="12" t="s">
         <v>64</v>
@@ -15607,11 +15595,8 @@
       <c r="A326" t="s">
         <v>1347</v>
       </c>
-      <c r="B326" s="7" t="s">
-        <v>1032</v>
-      </c>
       <c r="C326" s="14" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="E326" s="12" t="s">
         <v>64</v>
@@ -15627,8 +15612,11 @@
       <c r="A327" t="s">
         <v>1347</v>
       </c>
+      <c r="B327" s="6" t="s">
+        <v>202</v>
+      </c>
       <c r="C327" s="14" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="E327" s="12" t="s">
         <v>64</v>
@@ -15648,7 +15636,7 @@
         <v>202</v>
       </c>
       <c r="C328" s="14" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="E328" s="12" t="s">
         <v>64</v>
@@ -15668,7 +15656,7 @@
         <v>202</v>
       </c>
       <c r="C329" s="14" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="E329" s="12" t="s">
         <v>64</v>
@@ -15688,7 +15676,7 @@
         <v>202</v>
       </c>
       <c r="C330" s="14" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="E330" s="12" t="s">
         <v>64</v>
@@ -15708,7 +15696,7 @@
         <v>202</v>
       </c>
       <c r="C331" s="14" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="E331" s="12" t="s">
         <v>64</v>
@@ -15724,11 +15712,11 @@
       <c r="A332" t="s">
         <v>1347</v>
       </c>
-      <c r="B332" s="6" t="s">
-        <v>202</v>
+      <c r="B332" s="8" t="s">
+        <v>324</v>
       </c>
       <c r="C332" s="14" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="E332" s="12" t="s">
         <v>64</v>
@@ -15748,7 +15736,7 @@
         <v>324</v>
       </c>
       <c r="C333" s="14" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="E333" s="12" t="s">
         <v>64</v>
@@ -15768,7 +15756,7 @@
         <v>324</v>
       </c>
       <c r="C334" s="14" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="E334" s="12" t="s">
         <v>64</v>
@@ -15788,7 +15776,7 @@
         <v>324</v>
       </c>
       <c r="C335" s="14" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="E335" s="12" t="s">
         <v>64</v>
@@ -15804,11 +15792,8 @@
       <c r="A336" t="s">
         <v>1347</v>
       </c>
-      <c r="B336" s="8" t="s">
-        <v>324</v>
-      </c>
       <c r="C336" s="14" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="E336" s="12" t="s">
         <v>64</v>
@@ -15825,7 +15810,7 @@
         <v>1347</v>
       </c>
       <c r="C337" s="14" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="E337" s="12" t="s">
         <v>64</v>
@@ -15841,8 +15826,11 @@
       <c r="A338" t="s">
         <v>1347</v>
       </c>
+      <c r="B338" s="6" t="s">
+        <v>202</v>
+      </c>
       <c r="C338" s="14" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="E338" s="12" t="s">
         <v>64</v>
@@ -15858,11 +15846,11 @@
       <c r="A339" t="s">
         <v>1347</v>
       </c>
-      <c r="B339" s="6" t="s">
-        <v>202</v>
+      <c r="B339" s="9" t="s">
+        <v>400</v>
       </c>
       <c r="C339" s="14" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="E339" s="12" t="s">
         <v>64</v>
@@ -15882,7 +15870,7 @@
         <v>400</v>
       </c>
       <c r="C340" s="14" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="E340" s="12" t="s">
         <v>64</v>
@@ -15902,7 +15890,7 @@
         <v>400</v>
       </c>
       <c r="C341" s="14" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="E341" s="12" t="s">
         <v>64</v>
@@ -15922,7 +15910,7 @@
         <v>400</v>
       </c>
       <c r="C342" s="14" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="E342" s="12" t="s">
         <v>64</v>
@@ -15936,13 +15924,13 @@
     </row>
     <row r="343" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>1347</v>
-      </c>
-      <c r="B343" s="9" t="s">
-        <v>400</v>
+        <v>1348</v>
+      </c>
+      <c r="B343" s="4" t="s">
+        <v>719</v>
       </c>
       <c r="C343" s="14" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="E343" s="12" t="s">
         <v>64</v>
@@ -15956,19 +15944,19 @@
     </row>
     <row r="344" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>1348</v>
-      </c>
-      <c r="B344" s="4" t="s">
-        <v>719</v>
+        <v>1351</v>
+      </c>
+      <c r="B344" s="5" t="s">
+        <v>827</v>
       </c>
       <c r="C344" s="14" t="s">
-        <v>1323</v>
-      </c>
-      <c r="E344" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F344" s="12" t="s">
-        <v>65</v>
+        <v>1324</v>
+      </c>
+      <c r="E344" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F344" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="N344" t="s">
         <v>160</v>
@@ -15981,17 +15969,32 @@
       <c r="B345" s="5" t="s">
         <v>827</v>
       </c>
-      <c r="C345" s="14" t="s">
-        <v>1324</v>
-      </c>
-      <c r="E345" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="F345" s="10" t="s">
-        <v>57</v>
+      <c r="C345" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="D345" t="s">
+        <v>829</v>
+      </c>
+      <c r="E345" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F345" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H345" t="s">
+        <v>58</v>
+      </c>
+      <c r="L345" t="s">
+        <v>830</v>
       </c>
       <c r="N345" t="s">
-        <v>160</v>
+        <v>83</v>
+      </c>
+      <c r="O345" t="s">
+        <v>831</v>
+      </c>
+      <c r="P345" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="346" spans="1:16" x14ac:dyDescent="0.25">
@@ -16002,10 +16005,10 @@
         <v>827</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>828</v>
+        <v>832</v>
       </c>
       <c r="D346" t="s">
-        <v>829</v>
+        <v>833</v>
       </c>
       <c r="E346" s="12" t="s">
         <v>64</v>
@@ -16017,16 +16020,13 @@
         <v>58</v>
       </c>
       <c r="L346" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="N346" t="s">
-        <v>83</v>
-      </c>
-      <c r="O346" t="s">
-        <v>831</v>
+        <v>160</v>
       </c>
       <c r="P346" t="s">
-        <v>376</v>
+        <v>430</v>
       </c>
     </row>
     <row r="347" spans="1:16" x14ac:dyDescent="0.25">
@@ -16037,10 +16037,10 @@
         <v>827</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>832</v>
+        <v>835</v>
       </c>
       <c r="D347" t="s">
-        <v>833</v>
+        <v>836</v>
       </c>
       <c r="E347" s="12" t="s">
         <v>64</v>
@@ -16052,13 +16052,10 @@
         <v>58</v>
       </c>
       <c r="L347" t="s">
-        <v>834</v>
+        <v>837</v>
       </c>
       <c r="N347" t="s">
-        <v>160</v>
-      </c>
-      <c r="P347" t="s">
-        <v>430</v>
+        <v>71</v>
       </c>
     </row>
     <row r="348" spans="1:16" x14ac:dyDescent="0.25">
@@ -16069,10 +16066,10 @@
         <v>827</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>835</v>
+        <v>838</v>
       </c>
       <c r="D348" t="s">
-        <v>836</v>
+        <v>839</v>
       </c>
       <c r="E348" s="12" t="s">
         <v>64</v>
@@ -16084,10 +16081,13 @@
         <v>58</v>
       </c>
       <c r="L348" t="s">
-        <v>837</v>
+        <v>840</v>
       </c>
       <c r="N348" t="s">
         <v>71</v>
+      </c>
+      <c r="P348" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="349" spans="1:16" x14ac:dyDescent="0.25">
@@ -16098,10 +16098,10 @@
         <v>827</v>
       </c>
       <c r="C349" s="1" t="s">
-        <v>838</v>
+        <v>841</v>
       </c>
       <c r="D349" t="s">
-        <v>839</v>
+        <v>842</v>
       </c>
       <c r="E349" s="12" t="s">
         <v>64</v>
@@ -16110,10 +16110,13 @@
         <v>65</v>
       </c>
       <c r="H349" t="s">
-        <v>58</v>
+        <v>295</v>
+      </c>
+      <c r="I349" t="s">
+        <v>843</v>
       </c>
       <c r="L349" t="s">
-        <v>840</v>
+        <v>844</v>
       </c>
       <c r="N349" t="s">
         <v>71</v>
@@ -16130,10 +16133,10 @@
         <v>827</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>841</v>
+        <v>845</v>
       </c>
       <c r="D350" t="s">
-        <v>842</v>
+        <v>846</v>
       </c>
       <c r="E350" s="12" t="s">
         <v>64</v>
@@ -16142,13 +16145,10 @@
         <v>65</v>
       </c>
       <c r="H350" t="s">
-        <v>295</v>
-      </c>
-      <c r="I350" t="s">
-        <v>843</v>
+        <v>58</v>
       </c>
       <c r="L350" t="s">
-        <v>844</v>
+        <v>847</v>
       </c>
       <c r="N350" t="s">
         <v>71</v>
@@ -16165,10 +16165,10 @@
         <v>827</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
       <c r="D351" t="s">
-        <v>846</v>
+        <v>849</v>
       </c>
       <c r="E351" s="12" t="s">
         <v>64</v>
@@ -16177,10 +16177,13 @@
         <v>65</v>
       </c>
       <c r="H351" t="s">
-        <v>58</v>
+        <v>295</v>
+      </c>
+      <c r="I351" t="s">
+        <v>843</v>
       </c>
       <c r="L351" t="s">
-        <v>847</v>
+        <v>850</v>
       </c>
       <c r="N351" t="s">
         <v>71</v>
@@ -16197,10 +16200,10 @@
         <v>827</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>848</v>
+        <v>851</v>
       </c>
       <c r="D352" t="s">
-        <v>849</v>
+        <v>852</v>
       </c>
       <c r="E352" s="12" t="s">
         <v>64</v>
@@ -16215,7 +16218,7 @@
         <v>843</v>
       </c>
       <c r="L352" t="s">
-        <v>850</v>
+        <v>853</v>
       </c>
       <c r="N352" t="s">
         <v>71</v>
@@ -16232,10 +16235,10 @@
         <v>827</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>851</v>
+        <v>854</v>
       </c>
       <c r="D353" t="s">
-        <v>852</v>
+        <v>855</v>
       </c>
       <c r="E353" s="12" t="s">
         <v>64</v>
@@ -16244,13 +16247,10 @@
         <v>65</v>
       </c>
       <c r="H353" t="s">
-        <v>295</v>
-      </c>
-      <c r="I353" t="s">
-        <v>843</v>
+        <v>58</v>
       </c>
       <c r="L353" t="s">
-        <v>853</v>
+        <v>856</v>
       </c>
       <c r="N353" t="s">
         <v>71</v>
@@ -16267,10 +16267,10 @@
         <v>827</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>854</v>
+        <v>857</v>
       </c>
       <c r="D354" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c r="E354" s="12" t="s">
         <v>64</v>
@@ -16282,7 +16282,7 @@
         <v>58</v>
       </c>
       <c r="L354" t="s">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="N354" t="s">
         <v>71</v>
@@ -16299,10 +16299,10 @@
         <v>827</v>
       </c>
       <c r="C355" s="1" t="s">
-        <v>857</v>
+        <v>860</v>
       </c>
       <c r="D355" t="s">
-        <v>858</v>
+        <v>861</v>
       </c>
       <c r="E355" s="12" t="s">
         <v>64</v>
@@ -16311,10 +16311,13 @@
         <v>65</v>
       </c>
       <c r="H355" t="s">
-        <v>58</v>
+        <v>100</v>
+      </c>
+      <c r="K355" t="s">
+        <v>862</v>
       </c>
       <c r="L355" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="N355" t="s">
         <v>71</v>
@@ -16331,10 +16334,10 @@
         <v>827</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>860</v>
+        <v>864</v>
       </c>
       <c r="D356" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="E356" s="12" t="s">
         <v>64</v>
@@ -16343,13 +16346,10 @@
         <v>65</v>
       </c>
       <c r="H356" t="s">
-        <v>100</v>
-      </c>
-      <c r="K356" t="s">
-        <v>862</v>
+        <v>118</v>
       </c>
       <c r="L356" t="s">
-        <v>863</v>
+        <v>866</v>
       </c>
       <c r="N356" t="s">
         <v>71</v>
@@ -16366,10 +16366,10 @@
         <v>827</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>864</v>
+        <v>867</v>
       </c>
       <c r="D357" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="E357" s="12" t="s">
         <v>64</v>
@@ -16378,16 +16378,19 @@
         <v>65</v>
       </c>
       <c r="H357" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
       <c r="L357" t="s">
-        <v>866</v>
+        <v>869</v>
       </c>
       <c r="N357" t="s">
-        <v>71</v>
+        <v>83</v>
+      </c>
+      <c r="O357" t="s">
+        <v>870</v>
       </c>
       <c r="P357" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
     </row>
     <row r="358" spans="1:16" x14ac:dyDescent="0.25">
@@ -16398,10 +16401,10 @@
         <v>827</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>867</v>
+        <v>871</v>
       </c>
       <c r="D358" t="s">
-        <v>868</v>
+        <v>872</v>
       </c>
       <c r="E358" s="12" t="s">
         <v>64</v>
@@ -16413,16 +16416,13 @@
         <v>58</v>
       </c>
       <c r="L358" t="s">
-        <v>869</v>
+        <v>873</v>
       </c>
       <c r="N358" t="s">
-        <v>83</v>
-      </c>
-      <c r="O358" t="s">
-        <v>870</v>
+        <v>71</v>
       </c>
       <c r="P358" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
     </row>
     <row r="359" spans="1:16" x14ac:dyDescent="0.25">
@@ -16433,10 +16433,10 @@
         <v>827</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>871</v>
+        <v>874</v>
       </c>
       <c r="D359" t="s">
-        <v>872</v>
+        <v>875</v>
       </c>
       <c r="E359" s="12" t="s">
         <v>64</v>
@@ -16448,7 +16448,7 @@
         <v>58</v>
       </c>
       <c r="L359" t="s">
-        <v>873</v>
+        <v>876</v>
       </c>
       <c r="N359" t="s">
         <v>71</v>
@@ -16465,10 +16465,10 @@
         <v>827</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>874</v>
+        <v>877</v>
       </c>
       <c r="D360" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="E360" s="12" t="s">
         <v>64</v>
@@ -16477,16 +16477,22 @@
         <v>65</v>
       </c>
       <c r="H360" t="s">
-        <v>58</v>
+        <v>118</v>
+      </c>
+      <c r="I360" t="s">
+        <v>682</v>
       </c>
       <c r="L360" t="s">
-        <v>876</v>
+        <v>879</v>
       </c>
       <c r="N360" t="s">
-        <v>71</v>
+        <v>83</v>
+      </c>
+      <c r="O360" t="s">
+        <v>880</v>
       </c>
       <c r="P360" t="s">
-        <v>72</v>
+        <v>376</v>
       </c>
     </row>
     <row r="361" spans="1:16" x14ac:dyDescent="0.25">
@@ -16497,10 +16503,10 @@
         <v>827</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>877</v>
+        <v>881</v>
       </c>
       <c r="D361" t="s">
-        <v>878</v>
+        <v>882</v>
       </c>
       <c r="E361" s="12" t="s">
         <v>64</v>
@@ -16509,22 +16515,22 @@
         <v>65</v>
       </c>
       <c r="H361" t="s">
-        <v>118</v>
+        <v>300</v>
       </c>
       <c r="I361" t="s">
-        <v>682</v>
+        <v>883</v>
+      </c>
+      <c r="K361" t="s">
+        <v>884</v>
       </c>
       <c r="L361" t="s">
-        <v>879</v>
+        <v>287</v>
       </c>
       <c r="N361" t="s">
-        <v>83</v>
-      </c>
-      <c r="O361" t="s">
-        <v>880</v>
+        <v>71</v>
       </c>
       <c r="P361" t="s">
-        <v>376</v>
+        <v>72</v>
       </c>
     </row>
     <row r="362" spans="1:16" x14ac:dyDescent="0.25">
@@ -16535,10 +16541,10 @@
         <v>827</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>881</v>
+        <v>885</v>
       </c>
       <c r="D362" t="s">
-        <v>882</v>
+        <v>886</v>
       </c>
       <c r="E362" s="12" t="s">
         <v>64</v>
@@ -16547,16 +16553,13 @@
         <v>65</v>
       </c>
       <c r="H362" t="s">
-        <v>300</v>
-      </c>
-      <c r="I362" t="s">
-        <v>883</v>
+        <v>100</v>
       </c>
       <c r="K362" t="s">
-        <v>884</v>
+        <v>887</v>
       </c>
       <c r="L362" t="s">
-        <v>287</v>
+        <v>682</v>
       </c>
       <c r="N362" t="s">
         <v>71</v>
@@ -16573,10 +16576,10 @@
         <v>827</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c r="D363" t="s">
-        <v>886</v>
+        <v>889</v>
       </c>
       <c r="E363" s="12" t="s">
         <v>64</v>
@@ -16585,13 +16588,10 @@
         <v>65</v>
       </c>
       <c r="H363" t="s">
-        <v>100</v>
-      </c>
-      <c r="K363" t="s">
-        <v>887</v>
+        <v>58</v>
       </c>
       <c r="L363" t="s">
-        <v>682</v>
+        <v>840</v>
       </c>
       <c r="N363" t="s">
         <v>71</v>
@@ -16608,28 +16608,31 @@
         <v>827</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="D364" t="s">
-        <v>889</v>
-      </c>
-      <c r="E364" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F364" s="12" t="s">
-        <v>65</v>
+        <v>891</v>
+      </c>
+      <c r="E364" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F364" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="H364" t="s">
         <v>58</v>
       </c>
       <c r="L364" t="s">
-        <v>840</v>
+        <v>892</v>
       </c>
       <c r="N364" t="s">
-        <v>71</v>
+        <v>83</v>
+      </c>
+      <c r="O364" t="s">
+        <v>893</v>
       </c>
       <c r="P364" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
     </row>
     <row r="365" spans="1:16" x14ac:dyDescent="0.25">
@@ -16640,31 +16643,28 @@
         <v>827</v>
       </c>
       <c r="C365" s="1" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="D365" t="s">
-        <v>891</v>
-      </c>
-      <c r="E365" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F365" s="11" t="s">
-        <v>106</v>
+        <v>895</v>
+      </c>
+      <c r="E365" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F365" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="H365" t="s">
         <v>58</v>
       </c>
       <c r="L365" t="s">
-        <v>892</v>
+        <v>896</v>
       </c>
       <c r="N365" t="s">
-        <v>83</v>
-      </c>
-      <c r="O365" t="s">
-        <v>893</v>
+        <v>71</v>
       </c>
       <c r="P365" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
     </row>
     <row r="366" spans="1:16" x14ac:dyDescent="0.25">
@@ -16675,22 +16675,25 @@
         <v>827</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
       <c r="D366" t="s">
-        <v>895</v>
-      </c>
-      <c r="E366" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="F366" s="13" t="s">
-        <v>93</v>
+        <v>898</v>
+      </c>
+      <c r="E366" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F366" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="H366" t="s">
-        <v>58</v>
+        <v>100</v>
+      </c>
+      <c r="K366" t="s">
+        <v>899</v>
       </c>
       <c r="L366" t="s">
-        <v>896</v>
+        <v>900</v>
       </c>
       <c r="N366" t="s">
         <v>71</v>
@@ -16707,10 +16710,10 @@
         <v>827</v>
       </c>
       <c r="C367" s="1" t="s">
-        <v>897</v>
+        <v>901</v>
       </c>
       <c r="D367" t="s">
-        <v>898</v>
+        <v>902</v>
       </c>
       <c r="E367" s="11" t="s">
         <v>105</v>
@@ -16719,19 +16722,19 @@
         <v>106</v>
       </c>
       <c r="H367" t="s">
-        <v>100</v>
-      </c>
-      <c r="K367" t="s">
-        <v>899</v>
+        <v>58</v>
       </c>
       <c r="L367" t="s">
-        <v>900</v>
+        <v>903</v>
       </c>
       <c r="N367" t="s">
-        <v>71</v>
+        <v>83</v>
+      </c>
+      <c r="O367" t="s">
+        <v>904</v>
       </c>
       <c r="P367" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
     </row>
     <row r="368" spans="1:16" x14ac:dyDescent="0.25">
@@ -16742,31 +16745,31 @@
         <v>827</v>
       </c>
       <c r="C368" s="1" t="s">
-        <v>901</v>
+        <v>905</v>
       </c>
       <c r="D368" t="s">
-        <v>902</v>
-      </c>
-      <c r="E368" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F368" s="11" t="s">
-        <v>106</v>
+        <v>906</v>
+      </c>
+      <c r="E368" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F368" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="H368" t="s">
-        <v>58</v>
+        <v>118</v>
+      </c>
+      <c r="I368" t="s">
+        <v>682</v>
       </c>
       <c r="L368" t="s">
-        <v>903</v>
+        <v>907</v>
       </c>
       <c r="N368" t="s">
-        <v>83</v>
-      </c>
-      <c r="O368" t="s">
-        <v>904</v>
+        <v>71</v>
       </c>
       <c r="P368" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
     </row>
     <row r="369" spans="1:16" x14ac:dyDescent="0.25">
@@ -16777,10 +16780,10 @@
         <v>827</v>
       </c>
       <c r="C369" s="1" t="s">
-        <v>905</v>
+        <v>908</v>
       </c>
       <c r="D369" t="s">
-        <v>906</v>
+        <v>909</v>
       </c>
       <c r="E369" s="12" t="s">
         <v>64</v>
@@ -16795,7 +16798,7 @@
         <v>682</v>
       </c>
       <c r="L369" t="s">
-        <v>907</v>
+        <v>910</v>
       </c>
       <c r="N369" t="s">
         <v>71</v>
@@ -16812,10 +16815,10 @@
         <v>827</v>
       </c>
       <c r="C370" s="1" t="s">
-        <v>908</v>
+        <v>911</v>
       </c>
       <c r="D370" t="s">
-        <v>909</v>
+        <v>912</v>
       </c>
       <c r="E370" s="12" t="s">
         <v>64</v>
@@ -16824,13 +16827,10 @@
         <v>65</v>
       </c>
       <c r="H370" t="s">
-        <v>118</v>
-      </c>
-      <c r="I370" t="s">
-        <v>682</v>
+        <v>58</v>
       </c>
       <c r="L370" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
       <c r="N370" t="s">
         <v>71</v>
@@ -16847,10 +16847,10 @@
         <v>827</v>
       </c>
       <c r="C371" s="1" t="s">
-        <v>911</v>
+        <v>914</v>
       </c>
       <c r="D371" t="s">
-        <v>912</v>
+        <v>915</v>
       </c>
       <c r="E371" s="12" t="s">
         <v>64</v>
@@ -16862,13 +16862,16 @@
         <v>58</v>
       </c>
       <c r="L371" t="s">
-        <v>913</v>
+        <v>916</v>
       </c>
       <c r="N371" t="s">
-        <v>71</v>
+        <v>83</v>
+      </c>
+      <c r="O371" t="s">
+        <v>917</v>
       </c>
       <c r="P371" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
     </row>
     <row r="372" spans="1:16" x14ac:dyDescent="0.25">
@@ -16879,31 +16882,31 @@
         <v>827</v>
       </c>
       <c r="C372" s="1" t="s">
-        <v>914</v>
+        <v>918</v>
       </c>
       <c r="D372" t="s">
-        <v>915</v>
-      </c>
-      <c r="E372" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F372" s="12" t="s">
-        <v>65</v>
+        <v>919</v>
+      </c>
+      <c r="E372" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F372" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G372" t="s">
+        <v>920</v>
       </c>
       <c r="H372" t="s">
         <v>58</v>
       </c>
       <c r="L372" t="s">
-        <v>916</v>
+        <v>921</v>
       </c>
       <c r="N372" t="s">
-        <v>83</v>
-      </c>
-      <c r="O372" t="s">
-        <v>917</v>
+        <v>71</v>
       </c>
       <c r="P372" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
     </row>
     <row r="373" spans="1:16" x14ac:dyDescent="0.25">
@@ -16914,25 +16917,25 @@
         <v>827</v>
       </c>
       <c r="C373" s="1" t="s">
-        <v>918</v>
+        <v>922</v>
       </c>
       <c r="D373" t="s">
-        <v>919</v>
-      </c>
-      <c r="E373" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F373" s="11" t="s">
-        <v>106</v>
+        <v>923</v>
+      </c>
+      <c r="E373" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F373" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="G373" t="s">
-        <v>920</v>
+        <v>924</v>
       </c>
       <c r="H373" t="s">
         <v>58</v>
       </c>
       <c r="L373" t="s">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c r="N373" t="s">
         <v>71</v>
@@ -16949,10 +16952,10 @@
         <v>827</v>
       </c>
       <c r="C374" s="1" t="s">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c r="D374" t="s">
-        <v>923</v>
+        <v>927</v>
       </c>
       <c r="E374" s="12" t="s">
         <v>64</v>
@@ -16961,13 +16964,13 @@
         <v>65</v>
       </c>
       <c r="G374" t="s">
-        <v>924</v>
+        <v>928</v>
       </c>
       <c r="H374" t="s">
         <v>58</v>
       </c>
       <c r="L374" t="s">
-        <v>925</v>
+        <v>929</v>
       </c>
       <c r="N374" t="s">
         <v>71</v>
@@ -16984,25 +16987,22 @@
         <v>827</v>
       </c>
       <c r="C375" s="1" t="s">
-        <v>926</v>
+        <v>930</v>
       </c>
       <c r="D375" t="s">
-        <v>927</v>
+        <v>931</v>
       </c>
       <c r="E375" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F375" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="G375" t="s">
-        <v>928</v>
       </c>
       <c r="H375" t="s">
         <v>58</v>
       </c>
       <c r="L375" t="s">
-        <v>929</v>
+        <v>916</v>
       </c>
       <c r="N375" t="s">
         <v>71</v>
@@ -17019,10 +17019,10 @@
         <v>827</v>
       </c>
       <c r="C376" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="D376" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="E376" s="12" t="s">
         <v>64</v>
@@ -17034,7 +17034,7 @@
         <v>58</v>
       </c>
       <c r="L376" t="s">
-        <v>916</v>
+        <v>934</v>
       </c>
       <c r="N376" t="s">
         <v>71</v>
@@ -17051,10 +17051,10 @@
         <v>827</v>
       </c>
       <c r="C377" s="1" t="s">
-        <v>932</v>
+        <v>935</v>
       </c>
       <c r="D377" t="s">
-        <v>933</v>
+        <v>936</v>
       </c>
       <c r="E377" s="12" t="s">
         <v>64</v>
@@ -17066,7 +17066,7 @@
         <v>58</v>
       </c>
       <c r="L377" t="s">
-        <v>934</v>
+        <v>937</v>
       </c>
       <c r="N377" t="s">
         <v>71</v>
@@ -17083,22 +17083,22 @@
         <v>827</v>
       </c>
       <c r="C378" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="D378" t="s">
-        <v>936</v>
-      </c>
-      <c r="E378" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F378" s="12" t="s">
-        <v>65</v>
+        <v>939</v>
+      </c>
+      <c r="E378" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F378" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="H378" t="s">
         <v>58</v>
       </c>
       <c r="L378" t="s">
-        <v>937</v>
+        <v>940</v>
       </c>
       <c r="N378" t="s">
         <v>71</v>
@@ -17115,28 +17115,34 @@
         <v>827</v>
       </c>
       <c r="C379" s="1" t="s">
-        <v>938</v>
+        <v>946</v>
       </c>
       <c r="D379" t="s">
-        <v>939</v>
-      </c>
-      <c r="E379" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="F379" s="13" t="s">
-        <v>93</v>
+        <v>947</v>
+      </c>
+      <c r="E379" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F379" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="H379" t="s">
-        <v>58</v>
+        <v>295</v>
+      </c>
+      <c r="I379" t="s">
+        <v>943</v>
       </c>
       <c r="L379" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="N379" t="s">
-        <v>71</v>
+        <v>125</v>
+      </c>
+      <c r="O379" t="s">
+        <v>949</v>
       </c>
       <c r="P379" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
     </row>
     <row r="380" spans="1:16" x14ac:dyDescent="0.25">
@@ -17147,10 +17153,10 @@
         <v>827</v>
       </c>
       <c r="C380" s="1" t="s">
-        <v>946</v>
+        <v>950</v>
       </c>
       <c r="D380" t="s">
-        <v>947</v>
+        <v>951</v>
       </c>
       <c r="E380" s="12" t="s">
         <v>64</v>
@@ -17161,20 +17167,14 @@
       <c r="H380" t="s">
         <v>295</v>
       </c>
-      <c r="I380" t="s">
-        <v>943</v>
-      </c>
       <c r="L380" t="s">
-        <v>948</v>
+        <v>952</v>
       </c>
       <c r="N380" t="s">
-        <v>125</v>
-      </c>
-      <c r="O380" t="s">
-        <v>949</v>
+        <v>71</v>
       </c>
       <c r="P380" t="s">
-        <v>39</v>
+        <v>953</v>
       </c>
     </row>
     <row r="381" spans="1:16" x14ac:dyDescent="0.25">
@@ -17185,10 +17185,10 @@
         <v>827</v>
       </c>
       <c r="C381" s="1" t="s">
-        <v>950</v>
+        <v>954</v>
       </c>
       <c r="D381" t="s">
-        <v>951</v>
+        <v>955</v>
       </c>
       <c r="E381" s="12" t="s">
         <v>64</v>
@@ -17200,7 +17200,7 @@
         <v>295</v>
       </c>
       <c r="L381" t="s">
-        <v>952</v>
+        <v>956</v>
       </c>
       <c r="N381" t="s">
         <v>71</v>
@@ -17216,11 +17216,8 @@
       <c r="B382" s="5" t="s">
         <v>827</v>
       </c>
-      <c r="C382" s="1" t="s">
-        <v>954</v>
-      </c>
-      <c r="D382" t="s">
-        <v>955</v>
+      <c r="C382" s="14" t="s">
+        <v>1325</v>
       </c>
       <c r="E382" s="12" t="s">
         <v>64</v>
@@ -17228,17 +17225,8 @@
       <c r="F382" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H382" t="s">
-        <v>295</v>
-      </c>
-      <c r="L382" t="s">
-        <v>956</v>
-      </c>
       <c r="N382" t="s">
-        <v>71</v>
-      </c>
-      <c r="P382" t="s">
-        <v>953</v>
+        <v>160</v>
       </c>
     </row>
     <row r="383" spans="1:16" x14ac:dyDescent="0.25">
@@ -17249,7 +17237,7 @@
         <v>827</v>
       </c>
       <c r="C383" s="14" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="E383" s="12" t="s">
         <v>64</v>
@@ -17269,7 +17257,7 @@
         <v>827</v>
       </c>
       <c r="C384" s="14" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="E384" s="12" t="s">
         <v>64</v>
@@ -17289,7 +17277,7 @@
         <v>827</v>
       </c>
       <c r="C385" s="14" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="E385" s="12" t="s">
         <v>64</v>
@@ -17309,7 +17297,7 @@
         <v>827</v>
       </c>
       <c r="C386" s="14" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="E386" s="12" t="s">
         <v>64</v>
@@ -17329,7 +17317,7 @@
         <v>827</v>
       </c>
       <c r="C387" s="14" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="E387" s="12" t="s">
         <v>64</v>
@@ -17349,7 +17337,7 @@
         <v>827</v>
       </c>
       <c r="C388" s="14" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="E388" s="12" t="s">
         <v>64</v>
@@ -17369,7 +17357,7 @@
         <v>827</v>
       </c>
       <c r="C389" s="14" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="E389" s="12" t="s">
         <v>64</v>
@@ -17389,7 +17377,7 @@
         <v>827</v>
       </c>
       <c r="C390" s="14" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="E390" s="12" t="s">
         <v>64</v>
@@ -17409,7 +17397,7 @@
         <v>827</v>
       </c>
       <c r="C391" s="14" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="E391" s="12" t="s">
         <v>64</v>
@@ -17429,7 +17417,7 @@
         <v>827</v>
       </c>
       <c r="C392" s="14" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="E392" s="12" t="s">
         <v>64</v>
@@ -17449,7 +17437,7 @@
         <v>827</v>
       </c>
       <c r="C393" s="14" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="E393" s="12" t="s">
         <v>64</v>
@@ -17469,7 +17457,7 @@
         <v>827</v>
       </c>
       <c r="C394" s="14" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="E394" s="12" t="s">
         <v>64</v>
@@ -17489,7 +17477,7 @@
         <v>827</v>
       </c>
       <c r="C395" s="14" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="E395" s="12" t="s">
         <v>64</v>
@@ -17509,7 +17497,7 @@
         <v>827</v>
       </c>
       <c r="C396" s="14" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="E396" s="12" t="s">
         <v>64</v>
@@ -17529,7 +17517,7 @@
         <v>827</v>
       </c>
       <c r="C397" s="14" t="s">
-        <v>1339</v>
+        <v>1357</v>
       </c>
       <c r="E397" s="12" t="s">
         <v>64</v>
@@ -17549,7 +17537,7 @@
         <v>827</v>
       </c>
       <c r="C398" s="14" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="E398" s="12" t="s">
         <v>64</v>
@@ -17569,7 +17557,7 @@
         <v>827</v>
       </c>
       <c r="C399" s="14" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="E399" s="12" t="s">
         <v>64</v>
@@ -17589,7 +17577,7 @@
         <v>827</v>
       </c>
       <c r="C400" s="14" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="E400" s="12" t="s">
         <v>64</v>
@@ -17609,7 +17597,7 @@
         <v>827</v>
       </c>
       <c r="C401" s="14" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="E401" s="12" t="s">
         <v>64</v>
@@ -17629,7 +17617,7 @@
         <v>827</v>
       </c>
       <c r="C402" s="14" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="E402" s="12" t="s">
         <v>64</v>
@@ -17649,7 +17637,7 @@
         <v>827</v>
       </c>
       <c r="C403" s="14" t="s">
-        <v>1353</v>
+        <v>1341</v>
       </c>
       <c r="E403" s="12" t="s">
         <v>64</v>
@@ -17669,7 +17657,7 @@
         <v>827</v>
       </c>
       <c r="C404" s="14" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="E404" s="12" t="s">
         <v>64</v>
@@ -17689,7 +17677,7 @@
         <v>827</v>
       </c>
       <c r="C405" s="14" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="E405" s="12" t="s">
         <v>64</v>
@@ -17709,7 +17697,7 @@
         <v>827</v>
       </c>
       <c r="C406" s="14" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="E406" s="12" t="s">
         <v>64</v>
@@ -17729,7 +17717,7 @@
         <v>827</v>
       </c>
       <c r="C407" s="14" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="E407" s="12" t="s">
         <v>64</v>
@@ -17749,7 +17737,7 @@
         <v>827</v>
       </c>
       <c r="C408" s="14" t="s">
-        <v>1345</v>
+        <v>1340</v>
       </c>
       <c r="E408" s="12" t="s">
         <v>64</v>
@@ -17758,26 +17746,6 @@
         <v>65</v>
       </c>
       <c r="N408" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="409" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A409" t="s">
-        <v>1351</v>
-      </c>
-      <c r="B409" s="5" t="s">
-        <v>827</v>
-      </c>
-      <c r="C409" s="14" t="s">
-        <v>1340</v>
-      </c>
-      <c r="E409" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F409" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="N409" t="s">
         <v>160</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New terms that we add get all the nice formatting and dropdowns that FAIReSheets originally did. ie anything that we add to the checklist will be inserted with proper formats
</commit_message>
<xml_diff>
--- a/input/FAIRe_NOAA_checklist_v1.0.xlsx
+++ b/input/FAIRe_NOAA_checklist_v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayden.willms\Documents\Code\FAIReSheets\FAIReSheets\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayde\OneDrive\Documents\NOAA_AOML_Code\FAIReSheets\FAIReSheets\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF30A36-85DD-4A43-B8A0-47BC61B311DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF5F9DE-229D-4C53-98ED-F180B03A5494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="2325" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6435" yWindow="2040" windowWidth="28140" windowHeight="12150" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4109" uniqueCount="1358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4125" uniqueCount="1365">
   <si>
     <t>Instructions for data submitters:</t>
   </si>
@@ -4095,6 +4095,27 @@
   </si>
   <si>
     <t>deblur_sample_stats</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>testing | test</t>
+  </si>
+  <si>
+    <t>testing | test | tester</t>
+  </si>
+  <si>
+    <t>testing stuff</t>
+  </si>
+  <si>
+    <t>also testing this</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test | testing</t>
   </si>
 </sst>
 </file>
@@ -4693,8 +4714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P408"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A272" workbookViewId="0">
-      <selection activeCell="D311" sqref="D311"/>
+    <sheetView tabSelected="1" topLeftCell="A287" workbookViewId="0">
+      <selection activeCell="D303" sqref="D303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15124,6 +15145,9 @@
       <c r="C302" s="1" t="s">
         <v>1282</v>
       </c>
+      <c r="D302" t="s">
+        <v>1358</v>
+      </c>
       <c r="E302" s="12" t="s">
         <v>64</v>
       </c>
@@ -15144,11 +15168,20 @@
       <c r="C303" s="1" t="s">
         <v>1283</v>
       </c>
+      <c r="D303" t="s">
+        <v>1362</v>
+      </c>
       <c r="E303" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F303" s="12" t="s">
         <v>65</v>
+      </c>
+      <c r="H303" t="s">
+        <v>100</v>
+      </c>
+      <c r="K303" t="s">
+        <v>1359</v>
       </c>
       <c r="N303" t="s">
         <v>160</v>
@@ -15204,6 +15237,9 @@
       <c r="C306" s="14" t="s">
         <v>1286</v>
       </c>
+      <c r="D306" t="s">
+        <v>1358</v>
+      </c>
       <c r="E306" s="12" t="s">
         <v>64</v>
       </c>
@@ -15224,11 +15260,20 @@
       <c r="C307" s="14" t="s">
         <v>1287</v>
       </c>
+      <c r="D307" t="s">
+        <v>1361</v>
+      </c>
       <c r="E307" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F307" s="12" t="s">
         <v>65</v>
+      </c>
+      <c r="H307" t="s">
+        <v>100</v>
+      </c>
+      <c r="K307" t="s">
+        <v>1360</v>
       </c>
       <c r="N307" t="s">
         <v>160</v>
@@ -15658,6 +15703,9 @@
       <c r="C329" s="14" t="s">
         <v>1309</v>
       </c>
+      <c r="D329" t="s">
+        <v>1362</v>
+      </c>
       <c r="E329" s="12" t="s">
         <v>64</v>
       </c>
@@ -15932,11 +15980,20 @@
       <c r="C343" s="14" t="s">
         <v>1323</v>
       </c>
+      <c r="D343" t="s">
+        <v>1358</v>
+      </c>
       <c r="E343" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F343" s="12" t="s">
         <v>65</v>
+      </c>
+      <c r="H343" t="s">
+        <v>100</v>
+      </c>
+      <c r="K343" t="s">
+        <v>1359</v>
       </c>
       <c r="N343" t="s">
         <v>160</v>
@@ -17339,6 +17396,9 @@
       <c r="C388" s="14" t="s">
         <v>1331</v>
       </c>
+      <c r="D388" t="s">
+        <v>1363</v>
+      </c>
       <c r="E388" s="12" t="s">
         <v>64</v>
       </c>
@@ -17559,11 +17619,20 @@
       <c r="C399" s="14" t="s">
         <v>1355</v>
       </c>
+      <c r="D399" t="s">
+        <v>1363</v>
+      </c>
       <c r="E399" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F399" s="12" t="s">
         <v>65</v>
+      </c>
+      <c r="H399" t="s">
+        <v>100</v>
+      </c>
+      <c r="K399" t="s">
+        <v>1364</v>
       </c>
       <c r="N399" t="s">
         <v>160</v>

</xml_diff>